<commit_message>
updated ModelUse and input-output example
</commit_message>
<xml_diff>
--- a/test_nf_input.xlsx
+++ b/test_nf_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zleady\Documents\StVrain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72A7DDB8-C216-4CFA-9C05-34DD3C15F3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE31EB91-22D3-438D-9CFD-E9D5DB45AD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="1770" windowWidth="21600" windowHeight="11325" xr2:uid="{3AF2E410-FAA3-4A9A-BC8E-FE890B70E349}"/>
+    <workbookView xWindow="3040" yWindow="1480" windowWidth="14400" windowHeight="7400" xr2:uid="{3AF2E410-FAA3-4A9A-BC8E-FE890B70E349}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -403,12 +403,12 @@
   <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2:D116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,1614 +422,1614 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1906</v>
       </c>
       <c r="B2" s="1">
-        <v>149314.22400000002</v>
+        <v>2763072</v>
       </c>
       <c r="C2" s="1">
-        <v>149314.22400000002</v>
+        <v>2763072</v>
       </c>
       <c r="D2" s="1">
-        <v>149314.22400000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2763072</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1907</v>
       </c>
       <c r="B3" s="1">
-        <v>189603.28580000001</v>
+        <v>3081437</v>
       </c>
       <c r="C3" s="1">
-        <v>189603.28580000001</v>
+        <v>3081437</v>
       </c>
       <c r="D3" s="1">
-        <v>189603.28580000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3081437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1908</v>
       </c>
       <c r="B4" s="1">
-        <v>91389.060300000012</v>
+        <v>1649464</v>
       </c>
       <c r="C4" s="1">
-        <v>91389.060300000012</v>
+        <v>1649464</v>
       </c>
       <c r="D4" s="1">
-        <v>91389.060300000012</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1649464</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1909</v>
       </c>
       <c r="B5" s="1">
-        <v>165939.353</v>
+        <v>3215703</v>
       </c>
       <c r="C5" s="1">
-        <v>165939.353</v>
+        <v>3215703</v>
       </c>
       <c r="D5" s="1">
-        <v>165939.353</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3215703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1910</v>
       </c>
       <c r="B6" s="1">
-        <v>76251.614300000001</v>
+        <v>1847184</v>
       </c>
       <c r="C6" s="1">
-        <v>76251.614300000001</v>
+        <v>1847184</v>
       </c>
       <c r="D6" s="1">
-        <v>76251.614300000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1847184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1911</v>
       </c>
       <c r="B7" s="1">
-        <v>100665.90400000001</v>
+        <v>2219891</v>
       </c>
       <c r="C7" s="1">
-        <v>100665.90400000001</v>
+        <v>2219891</v>
       </c>
       <c r="D7" s="1">
-        <v>100665.90400000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2219891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1912</v>
       </c>
       <c r="B8" s="1">
-        <v>152613.1882</v>
+        <v>2996054</v>
       </c>
       <c r="C8" s="1">
-        <v>152613.1882</v>
+        <v>2996054</v>
       </c>
       <c r="D8" s="1">
-        <v>152613.1882</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2996054</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1913</v>
       </c>
       <c r="B9" s="1">
-        <v>105020.36300000001</v>
+        <v>1830144</v>
       </c>
       <c r="C9" s="1">
-        <v>105020.36300000001</v>
+        <v>1830144</v>
       </c>
       <c r="D9" s="1">
-        <v>105020.36300000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1830144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1914</v>
       </c>
       <c r="B10" s="1">
-        <v>181326.55600000001</v>
+        <v>3086464</v>
       </c>
       <c r="C10" s="1">
-        <v>181326.55600000001</v>
+        <v>3086464</v>
       </c>
       <c r="D10" s="1">
-        <v>181326.55600000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3086464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1915</v>
       </c>
       <c r="B11" s="1">
-        <v>146191.17560000002</v>
+        <v>1777819</v>
       </c>
       <c r="C11" s="1">
-        <v>146191.17560000002</v>
+        <v>1777819</v>
       </c>
       <c r="D11" s="1">
-        <v>146191.17560000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1777819</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1916</v>
       </c>
       <c r="B12" s="1">
-        <v>122891.01930000001</v>
+        <v>2342408</v>
       </c>
       <c r="C12" s="1">
-        <v>122891.01930000001</v>
+        <v>2342408</v>
       </c>
       <c r="D12" s="1">
-        <v>122891.01930000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2342408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1917</v>
       </c>
       <c r="B13" s="1">
-        <v>157272.78510000001</v>
+        <v>3030560</v>
       </c>
       <c r="C13" s="1">
-        <v>157272.78510000001</v>
+        <v>3030560</v>
       </c>
       <c r="D13" s="1">
-        <v>157272.78510000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3030560</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1918</v>
       </c>
       <c r="B14" s="1">
-        <v>135125.85460000002</v>
+        <v>2873726</v>
       </c>
       <c r="C14" s="1">
-        <v>135125.85460000002</v>
+        <v>2873726</v>
       </c>
       <c r="D14" s="1">
-        <v>135125.85460000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2873726</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1919</v>
       </c>
       <c r="B15" s="1">
-        <v>90051.231500000009</v>
+        <v>1669828</v>
       </c>
       <c r="C15" s="1">
-        <v>90051.231500000009</v>
+        <v>1669828</v>
       </c>
       <c r="D15" s="1">
-        <v>90051.231500000009</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1669828</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1920</v>
       </c>
       <c r="B16" s="1">
-        <v>137384.52660000001</v>
+        <v>2856653</v>
       </c>
       <c r="C16" s="1">
-        <v>137384.52660000001</v>
+        <v>2856653</v>
       </c>
       <c r="D16" s="1">
-        <v>137384.52660000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2856653</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1921</v>
       </c>
       <c r="B17" s="1">
-        <v>178934.31830000001</v>
+        <v>2980645</v>
       </c>
       <c r="C17" s="1">
-        <v>178934.31830000001</v>
+        <v>2980645</v>
       </c>
       <c r="D17" s="1">
-        <v>178934.31830000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2980645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1922</v>
       </c>
       <c r="B18" s="1">
-        <v>83579.267500000002</v>
+        <v>2050647</v>
       </c>
       <c r="C18" s="1">
-        <v>83579.267500000002</v>
+        <v>2050647</v>
       </c>
       <c r="D18" s="1">
-        <v>83579.267500000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2050647</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1923</v>
       </c>
       <c r="B19" s="1">
-        <v>188991.9241</v>
+        <v>2678876</v>
       </c>
       <c r="C19" s="1">
-        <v>188991.9241</v>
+        <v>2678876</v>
       </c>
       <c r="D19" s="1">
-        <v>188991.9241</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2678876</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1924</v>
       </c>
       <c r="B20" s="1">
-        <v>157746.23750000002</v>
+        <v>2236428</v>
       </c>
       <c r="C20" s="1">
-        <v>157746.23750000002</v>
+        <v>2236428</v>
       </c>
       <c r="D20" s="1">
-        <v>157746.23750000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2236428</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1925</v>
       </c>
       <c r="B21" s="1">
-        <v>84042.946800000005</v>
+        <v>1898141</v>
       </c>
       <c r="C21" s="1">
-        <v>84042.946800000005</v>
+        <v>1898141</v>
       </c>
       <c r="D21" s="1">
-        <v>84042.946800000005</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1898141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1926</v>
       </c>
       <c r="B22" s="1">
-        <v>166219.51520000002</v>
+        <v>2652645</v>
       </c>
       <c r="C22" s="1">
-        <v>166219.51520000002</v>
+        <v>2652645</v>
       </c>
       <c r="D22" s="1">
-        <v>166219.51520000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2652645</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1927</v>
       </c>
       <c r="B23" s="1">
-        <v>116768.7151</v>
+        <v>2538119</v>
       </c>
       <c r="C23" s="1">
-        <v>116768.7151</v>
+        <v>2538119</v>
       </c>
       <c r="D23" s="1">
-        <v>116768.7151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2538119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1928</v>
       </c>
       <c r="B24" s="1">
-        <v>131669.43489999999</v>
+        <v>2864621</v>
       </c>
       <c r="C24" s="1">
-        <v>131669.43489999999</v>
+        <v>2864621</v>
       </c>
       <c r="D24" s="1">
-        <v>131669.43489999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2864621</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1929</v>
       </c>
       <c r="B25" s="1">
-        <v>118332.41110000001</v>
+        <v>2888004</v>
       </c>
       <c r="C25" s="1">
-        <v>118332.41110000001</v>
+        <v>2888004</v>
       </c>
       <c r="D25" s="1">
-        <v>118332.41110000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2888004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1930</v>
       </c>
       <c r="B26" s="1">
-        <v>101924.4621</v>
+        <v>2132801</v>
       </c>
       <c r="C26" s="1">
-        <v>101924.4621</v>
+        <v>2132801</v>
       </c>
       <c r="D26" s="1">
-        <v>101924.4621</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2132801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1931</v>
       </c>
       <c r="B27" s="1">
-        <v>88437.584100000007</v>
+        <v>1286149</v>
       </c>
       <c r="C27" s="1">
-        <v>88437.584100000007</v>
+        <v>1286149</v>
       </c>
       <c r="D27" s="1">
-        <v>88437.584100000007</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1286149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1932</v>
       </c>
       <c r="B28" s="1">
-        <v>95030.082999999999</v>
+        <v>2134236</v>
       </c>
       <c r="C28" s="1">
-        <v>95030.082999999999</v>
+        <v>2134236</v>
       </c>
       <c r="D28" s="1">
-        <v>95030.082999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2134236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1933</v>
       </c>
       <c r="B29" s="1">
-        <v>130105.73890000001</v>
+        <v>2030154</v>
       </c>
       <c r="C29" s="1">
-        <v>130105.73890000001</v>
+        <v>2030154</v>
       </c>
       <c r="D29" s="1">
-        <v>130105.73890000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2030154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1934</v>
       </c>
       <c r="B30" s="1">
-        <v>82774.615600000005</v>
+        <v>1073765</v>
       </c>
       <c r="C30" s="1">
-        <v>82774.615600000005</v>
+        <v>1073765</v>
       </c>
       <c r="D30" s="1">
-        <v>82774.615600000005</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1073765</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1935</v>
       </c>
       <c r="B31" s="1">
-        <v>120467.2905</v>
+        <v>1737323</v>
       </c>
       <c r="C31" s="1">
-        <v>120467.2905</v>
+        <v>1737323</v>
       </c>
       <c r="D31" s="1">
-        <v>120467.2905</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1737323</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1936</v>
       </c>
       <c r="B32" s="1">
-        <v>139578.04460000002</v>
+        <v>2416056</v>
       </c>
       <c r="C32" s="1">
-        <v>139578.04460000002</v>
+        <v>2416056</v>
       </c>
       <c r="D32" s="1">
-        <v>139578.04460000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2416056</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1937</v>
       </c>
       <c r="B33" s="1">
-        <v>101749.63220000001</v>
+        <v>1569991</v>
       </c>
       <c r="C33" s="1">
-        <v>101749.63220000001</v>
+        <v>1569991</v>
       </c>
       <c r="D33" s="1">
-        <v>101749.63220000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1569991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1938</v>
       </c>
       <c r="B34" s="1">
-        <v>147257.5294</v>
+        <v>2584735</v>
       </c>
       <c r="C34" s="1">
-        <v>147257.5294</v>
+        <v>2584735</v>
       </c>
       <c r="D34" s="1">
-        <v>147257.5294</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2584735</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1939</v>
       </c>
       <c r="B35" s="1">
-        <v>88014.083100000003</v>
+        <v>1816650</v>
       </c>
       <c r="C35" s="1">
-        <v>88014.083100000003</v>
+        <v>1816650</v>
       </c>
       <c r="D35" s="1">
-        <v>88014.083100000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1816650</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1940</v>
       </c>
       <c r="B36" s="1">
-        <v>82216.463000000003</v>
+        <v>1471054</v>
       </c>
       <c r="C36" s="1">
-        <v>82216.463000000003</v>
+        <v>1471054</v>
       </c>
       <c r="D36" s="1">
-        <v>82216.463000000003</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1471054</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1941</v>
       </c>
       <c r="B37" s="1">
-        <v>117055.39270000001</v>
+        <v>1839369</v>
       </c>
       <c r="C37" s="1">
-        <v>117055.39270000001</v>
+        <v>1839369</v>
       </c>
       <c r="D37" s="1">
-        <v>117055.39270000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1839369</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1942</v>
       </c>
       <c r="B38" s="1">
-        <v>164776.35410000003</v>
+        <v>2021150</v>
       </c>
       <c r="C38" s="1">
-        <v>164776.35410000003</v>
+        <v>2021150</v>
       </c>
       <c r="D38" s="1">
-        <v>164776.35410000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2021150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1943</v>
       </c>
       <c r="B39" s="1">
-        <v>127189.01150000001</v>
+        <v>1992275</v>
       </c>
       <c r="C39" s="1">
-        <v>127189.01150000001</v>
+        <v>1992275</v>
       </c>
       <c r="D39" s="1">
-        <v>127189.01150000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1992275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1944</v>
       </c>
       <c r="B40" s="1">
-        <v>111067.74010000001</v>
+        <v>1618095</v>
       </c>
       <c r="C40" s="1">
-        <v>111067.74010000001</v>
+        <v>1618095</v>
       </c>
       <c r="D40" s="1">
-        <v>111067.74010000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1618095</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1945</v>
       </c>
       <c r="B41" s="1">
-        <v>121641.14840000001</v>
+        <v>1930815</v>
       </c>
       <c r="C41" s="1">
-        <v>121641.14840000001</v>
+        <v>1930815</v>
       </c>
       <c r="D41" s="1">
-        <v>121641.14840000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1930815</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1946</v>
       </c>
       <c r="B42" s="1">
-        <v>87481.992100000003</v>
+        <v>1689839</v>
       </c>
       <c r="C42" s="1">
-        <v>87481.992100000003</v>
+        <v>1689839</v>
       </c>
       <c r="D42" s="1">
-        <v>87481.992100000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1689839</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1947</v>
       </c>
       <c r="B43" s="1">
-        <v>168105.72350000002</v>
+        <v>2444252</v>
       </c>
       <c r="C43" s="1">
-        <v>168105.72350000002</v>
+        <v>2444252</v>
       </c>
       <c r="D43" s="1">
-        <v>168105.72350000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2444252</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1948</v>
       </c>
       <c r="B44" s="1">
-        <v>97201.883000000002</v>
+        <v>1993700</v>
       </c>
       <c r="C44" s="1">
-        <v>97201.883000000002</v>
+        <v>1993700</v>
       </c>
       <c r="D44" s="1">
-        <v>97201.883000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1993700</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1949</v>
       </c>
       <c r="B45" s="1">
-        <v>156130.41830000002</v>
+        <v>2197475</v>
       </c>
       <c r="C45" s="1">
-        <v>156130.41830000002</v>
+        <v>2197475</v>
       </c>
       <c r="D45" s="1">
-        <v>156130.41830000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2197475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1950</v>
       </c>
       <c r="B46" s="1">
-        <v>90694</v>
+        <v>1651854</v>
       </c>
       <c r="C46" s="1">
-        <v>90694</v>
+        <v>1651854</v>
       </c>
       <c r="D46" s="1">
-        <v>90694</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1651854</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1951</v>
       </c>
       <c r="B47" s="1">
-        <v>146893</v>
+        <v>2280116</v>
       </c>
       <c r="C47" s="1">
-        <v>146893</v>
+        <v>2280116</v>
       </c>
       <c r="D47" s="1">
-        <v>146893</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2280116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1952</v>
       </c>
       <c r="B48" s="1">
-        <v>155956</v>
+        <v>2857223</v>
       </c>
       <c r="C48" s="1">
-        <v>155956</v>
+        <v>2857223</v>
       </c>
       <c r="D48" s="1">
-        <v>155956</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2857223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1953</v>
       </c>
       <c r="B49" s="1">
-        <v>92631</v>
+        <v>1881901</v>
       </c>
       <c r="C49" s="1">
-        <v>92631</v>
+        <v>1881901</v>
       </c>
       <c r="D49" s="1">
-        <v>92631</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1881901</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1954</v>
       </c>
       <c r="B50" s="1">
-        <v>50159</v>
+        <v>1050069</v>
       </c>
       <c r="C50" s="1">
-        <v>50159</v>
+        <v>1050069</v>
       </c>
       <c r="D50" s="1">
-        <v>50159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1050069</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1955</v>
       </c>
       <c r="B51" s="1">
-        <v>72362</v>
+        <v>1408317</v>
       </c>
       <c r="C51" s="1">
-        <v>72362</v>
+        <v>1408317</v>
       </c>
       <c r="D51" s="1">
-        <v>72362</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1408317</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1956</v>
       </c>
       <c r="B52" s="1">
-        <v>81751</v>
+        <v>1869820</v>
       </c>
       <c r="C52" s="1">
-        <v>81751</v>
+        <v>1869820</v>
       </c>
       <c r="D52" s="1">
-        <v>81751</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1869820</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1957</v>
       </c>
       <c r="B53" s="1">
-        <v>186659</v>
+        <v>3096986</v>
       </c>
       <c r="C53" s="1">
-        <v>186659</v>
+        <v>3096986</v>
       </c>
       <c r="D53" s="1">
-        <v>186659</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3096986</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1958</v>
       </c>
       <c r="B54" s="1">
-        <v>104350</v>
+        <v>2000325</v>
       </c>
       <c r="C54" s="1">
-        <v>104350</v>
+        <v>2000325</v>
       </c>
       <c r="D54" s="1">
-        <v>104350</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2000325</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1959</v>
       </c>
       <c r="B55" s="1">
-        <v>109542</v>
+        <v>1789641</v>
       </c>
       <c r="C55" s="1">
-        <v>109542</v>
+        <v>1789641</v>
       </c>
       <c r="D55" s="1">
-        <v>109542</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1789641</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1960</v>
       </c>
       <c r="B56" s="1">
-        <v>98423</v>
+        <v>1919528</v>
       </c>
       <c r="C56" s="1">
-        <v>98423</v>
+        <v>1919528</v>
       </c>
       <c r="D56" s="1">
-        <v>98423</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1919528</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1961</v>
       </c>
       <c r="B57" s="1">
-        <v>128129</v>
+        <v>1664559</v>
       </c>
       <c r="C57" s="1">
-        <v>128129</v>
+        <v>1664559</v>
       </c>
       <c r="D57" s="1">
-        <v>128129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1664559</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1962</v>
       </c>
       <c r="B58" s="1">
-        <v>87655</v>
+        <v>2711854</v>
       </c>
       <c r="C58" s="1">
-        <v>87655</v>
+        <v>2711854</v>
       </c>
       <c r="D58" s="1">
-        <v>87655</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2711854</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1963</v>
       </c>
       <c r="B59" s="1">
-        <v>80636</v>
+        <v>1270052</v>
       </c>
       <c r="C59" s="1">
-        <v>80636</v>
+        <v>1270052</v>
       </c>
       <c r="D59" s="1">
-        <v>80636</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1270052</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1964</v>
       </c>
       <c r="B60" s="1">
-        <v>66100</v>
+        <v>1479570</v>
       </c>
       <c r="C60" s="1">
-        <v>66100</v>
+        <v>1479570</v>
       </c>
       <c r="D60" s="1">
-        <v>66100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1479570</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1965</v>
       </c>
       <c r="B61" s="1">
-        <v>139277</v>
+        <v>2578312</v>
       </c>
       <c r="C61" s="1">
-        <v>139277</v>
+        <v>2578312</v>
       </c>
       <c r="D61" s="1">
-        <v>139277</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2578312</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1966</v>
       </c>
       <c r="B62" s="1">
-        <v>54837</v>
+        <v>1257925</v>
       </c>
       <c r="C62" s="1">
-        <v>54837</v>
+        <v>1257925</v>
       </c>
       <c r="D62" s="1">
-        <v>54837</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1257925</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1967</v>
       </c>
       <c r="B63" s="1">
-        <v>105513</v>
+        <v>1765179</v>
       </c>
       <c r="C63" s="1">
-        <v>105513</v>
+        <v>1765179</v>
       </c>
       <c r="D63" s="1">
-        <v>105513</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1765179</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1968</v>
       </c>
       <c r="B64" s="1">
-        <v>87466</v>
+        <v>1844385</v>
       </c>
       <c r="C64" s="1">
-        <v>87466</v>
+        <v>1844385</v>
       </c>
       <c r="D64" s="1">
-        <v>87466</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1844385</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1969</v>
       </c>
       <c r="B65" s="1">
-        <v>176038</v>
+        <v>1987677</v>
       </c>
       <c r="C65" s="1">
-        <v>176038</v>
+        <v>1987677</v>
       </c>
       <c r="D65" s="1">
-        <v>176038</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1987677</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1970</v>
       </c>
       <c r="B66" s="1">
-        <v>125580</v>
+        <v>2429275</v>
       </c>
       <c r="C66" s="1">
-        <v>125580</v>
+        <v>2429275</v>
       </c>
       <c r="D66" s="1">
-        <v>125580</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2429275</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1971</v>
       </c>
       <c r="B67" s="1">
-        <v>133536</v>
+        <v>2499629</v>
       </c>
       <c r="C67" s="1">
-        <v>133536</v>
+        <v>2499629</v>
       </c>
       <c r="D67" s="1">
-        <v>133536</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2499629</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1972</v>
       </c>
       <c r="B68" s="1">
-        <v>94514</v>
+        <v>2022348</v>
       </c>
       <c r="C68" s="1">
-        <v>94514</v>
+        <v>2022348</v>
       </c>
       <c r="D68" s="1">
-        <v>94514</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2022348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1973</v>
       </c>
       <c r="B69" s="1">
-        <v>132203</v>
+        <v>2344794</v>
       </c>
       <c r="C69" s="1">
-        <v>132203</v>
+        <v>2344794</v>
       </c>
       <c r="D69" s="1">
-        <v>132203</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2344794</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1974</v>
       </c>
       <c r="B70" s="1">
-        <v>100168</v>
+        <v>2366549</v>
       </c>
       <c r="C70" s="1">
-        <v>100168</v>
+        <v>2366549</v>
       </c>
       <c r="D70" s="1">
-        <v>100168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2366549</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1975</v>
       </c>
       <c r="B71" s="1">
-        <v>121000</v>
+        <v>2150362</v>
       </c>
       <c r="C71" s="1">
-        <v>121000</v>
+        <v>2150362</v>
       </c>
       <c r="D71" s="1">
-        <v>121000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2150362</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1976</v>
       </c>
       <c r="B72" s="1">
-        <v>81623</v>
+        <v>1684210</v>
       </c>
       <c r="C72" s="1">
-        <v>81623</v>
+        <v>1684210</v>
       </c>
       <c r="D72" s="1">
-        <v>81623</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1684210</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1977</v>
       </c>
       <c r="B73" s="1">
-        <v>64023</v>
+        <v>1069044</v>
       </c>
       <c r="C73" s="1">
-        <v>64023</v>
+        <v>1069044</v>
       </c>
       <c r="D73" s="1">
-        <v>64023</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1069044</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1978</v>
       </c>
       <c r="B74" s="1">
-        <v>133230</v>
+        <v>2488953</v>
       </c>
       <c r="C74" s="1">
-        <v>133230</v>
+        <v>2488953</v>
       </c>
       <c r="D74" s="1">
-        <v>133230</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2488953</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1979</v>
       </c>
       <c r="B75" s="1">
-        <v>154206</v>
+        <v>2441731</v>
       </c>
       <c r="C75" s="1">
-        <v>154206</v>
+        <v>2441731</v>
       </c>
       <c r="D75" s="1">
-        <v>154206</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2441731</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1980</v>
       </c>
       <c r="B76" s="1">
-        <v>178824</v>
+        <v>2204962</v>
       </c>
       <c r="C76" s="1">
-        <v>178824</v>
+        <v>2204962</v>
       </c>
       <c r="D76" s="1">
-        <v>178824</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2204962</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1981</v>
       </c>
       <c r="B77" s="1">
-        <v>64145</v>
+        <v>1260614</v>
       </c>
       <c r="C77" s="1">
-        <v>64145</v>
+        <v>1260614</v>
       </c>
       <c r="D77" s="1">
-        <v>64145</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1260614</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1982</v>
       </c>
       <c r="B78" s="1">
-        <v>126776</v>
+        <v>2249838</v>
       </c>
       <c r="C78" s="1">
-        <v>126776</v>
+        <v>2249838</v>
       </c>
       <c r="D78" s="1">
-        <v>126776</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2249838</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1983</v>
       </c>
       <c r="B79" s="1">
-        <v>176515</v>
+        <v>2988820</v>
       </c>
       <c r="C79" s="1">
-        <v>176515</v>
+        <v>2988820</v>
       </c>
       <c r="D79" s="1">
-        <v>176515</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2988820</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1984</v>
       </c>
       <c r="B80" s="1">
-        <v>174671</v>
+        <v>3510442</v>
       </c>
       <c r="C80" s="1">
-        <v>174671</v>
+        <v>3510442</v>
       </c>
       <c r="D80" s="1">
-        <v>174671</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3510442</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1985</v>
       </c>
       <c r="B81" s="1">
-        <v>107155</v>
+        <v>2651302</v>
       </c>
       <c r="C81" s="1">
-        <v>107155</v>
+        <v>2651302</v>
       </c>
       <c r="D81" s="1">
-        <v>107155</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2651302</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1986</v>
       </c>
       <c r="B82" s="1">
-        <v>143784</v>
+        <v>2815896</v>
       </c>
       <c r="C82" s="1">
-        <v>143784</v>
+        <v>2815896</v>
       </c>
       <c r="D82" s="1">
-        <v>143784</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2815896</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1987</v>
       </c>
       <c r="B83" s="1">
-        <v>103297</v>
+        <v>1546120</v>
       </c>
       <c r="C83" s="1">
-        <v>103297</v>
+        <v>1546120</v>
       </c>
       <c r="D83" s="1">
-        <v>103297</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1546120</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1988</v>
       </c>
       <c r="B84" s="1">
-        <v>97519</v>
+        <v>1860724</v>
       </c>
       <c r="C84" s="1">
-        <v>97519</v>
+        <v>1860724</v>
       </c>
       <c r="D84" s="1">
-        <v>97519</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1860724</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1989</v>
       </c>
       <c r="B85" s="1">
-        <v>92790</v>
+        <v>1579420</v>
       </c>
       <c r="C85" s="1">
-        <v>92790</v>
+        <v>1579420</v>
       </c>
       <c r="D85" s="1">
-        <v>92790</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1579420</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1990</v>
       </c>
       <c r="B86" s="1">
-        <v>126911</v>
+        <v>1523544</v>
       </c>
       <c r="C86" s="1">
-        <v>126911</v>
+        <v>1523544</v>
       </c>
       <c r="D86" s="1">
-        <v>126911</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1523544</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1991</v>
       </c>
       <c r="B87" s="1">
-        <v>120178</v>
+        <v>1855396</v>
       </c>
       <c r="C87" s="1">
-        <v>120178</v>
+        <v>1855396</v>
       </c>
       <c r="D87" s="1">
-        <v>120178</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1855396</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1992</v>
       </c>
       <c r="B88" s="1">
-        <v>94891</v>
+        <v>1604988</v>
       </c>
       <c r="C88" s="1">
-        <v>94891</v>
+        <v>1604988</v>
       </c>
       <c r="D88" s="1">
-        <v>94891</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1604988</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1993</v>
       </c>
       <c r="B89" s="1">
-        <v>118834</v>
+        <v>2489636</v>
       </c>
       <c r="C89" s="1">
-        <v>118834</v>
+        <v>2489636</v>
       </c>
       <c r="D89" s="1">
-        <v>118834</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2489636</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1994</v>
       </c>
       <c r="B90" s="1">
-        <v>93891</v>
+        <v>1558779</v>
       </c>
       <c r="C90" s="1">
-        <v>93891</v>
+        <v>1558779</v>
       </c>
       <c r="D90" s="1">
-        <v>93891</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1558779</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1995</v>
       </c>
       <c r="B91" s="1">
-        <v>189492</v>
+        <v>2536548</v>
       </c>
       <c r="C91" s="1">
-        <v>189492</v>
+        <v>2536548</v>
       </c>
       <c r="D91" s="1">
-        <v>189492</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2536548</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1996</v>
       </c>
       <c r="B92" s="1">
-        <v>141562</v>
+        <v>2520216</v>
       </c>
       <c r="C92" s="1">
-        <v>141562</v>
+        <v>2520216</v>
       </c>
       <c r="D92" s="1">
-        <v>141562</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2520216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1997</v>
       </c>
       <c r="B93" s="1">
-        <v>169752</v>
+        <v>2961123</v>
       </c>
       <c r="C93" s="1">
-        <v>169752</v>
+        <v>2961123</v>
       </c>
       <c r="D93" s="1">
-        <v>169752</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2961123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1998</v>
       </c>
       <c r="B94" s="1">
-        <v>128419</v>
+        <v>1889077</v>
       </c>
       <c r="C94" s="1">
-        <v>128419</v>
+        <v>1889077</v>
       </c>
       <c r="D94" s="1">
-        <v>128419</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1889077</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1999</v>
       </c>
       <c r="B95" s="1">
-        <v>147073</v>
+        <v>2067493</v>
       </c>
       <c r="C95" s="1">
-        <v>147073</v>
+        <v>2067493</v>
       </c>
       <c r="D95" s="1">
-        <v>147073</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2067493</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2000</v>
       </c>
       <c r="B96" s="1">
-        <v>97996</v>
+        <v>1812552</v>
       </c>
       <c r="C96" s="1">
-        <v>97996</v>
+        <v>1812552</v>
       </c>
       <c r="D96" s="1">
-        <v>97996</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1812552</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2001</v>
       </c>
       <c r="B97" s="1">
-        <v>84163</v>
+        <v>1574117</v>
       </c>
       <c r="C97" s="1">
-        <v>84163</v>
+        <v>1574117</v>
       </c>
       <c r="D97" s="1">
-        <v>84163</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1574117</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2002</v>
       </c>
       <c r="B98" s="1">
-        <v>47348</v>
+        <v>891912</v>
       </c>
       <c r="C98" s="1">
-        <v>47348</v>
+        <v>891912</v>
       </c>
       <c r="D98" s="1">
-        <v>47348</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>891912</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2003</v>
       </c>
       <c r="B99" s="1">
-        <v>128537</v>
+        <v>2001412</v>
       </c>
       <c r="C99" s="1">
-        <v>128537</v>
+        <v>2001412</v>
       </c>
       <c r="D99" s="1">
-        <v>128537</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2001412</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2004</v>
       </c>
       <c r="B100" s="1">
-        <v>105346</v>
+        <v>1307362</v>
       </c>
       <c r="C100" s="1">
-        <v>105346</v>
+        <v>1307362</v>
       </c>
       <c r="D100" s="1">
-        <v>105346</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1307362</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2005</v>
       </c>
       <c r="B101" s="1">
-        <v>115218</v>
+        <v>1937400</v>
       </c>
       <c r="C101" s="1">
-        <v>115218</v>
+        <v>1937400</v>
       </c>
       <c r="D101" s="1">
-        <v>115218</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1937400</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2006</v>
       </c>
       <c r="B102" s="1">
-        <v>95202</v>
+        <v>2055498</v>
       </c>
       <c r="C102" s="1">
-        <v>95202</v>
+        <v>2055498</v>
       </c>
       <c r="D102" s="1">
-        <v>95202</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2055498</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2007</v>
       </c>
       <c r="B103" s="1">
-        <v>99494</v>
+        <v>1852090</v>
       </c>
       <c r="C103" s="1">
-        <v>99494</v>
+        <v>1852090</v>
       </c>
       <c r="D103" s="1">
-        <v>99494</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1852090</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2008</v>
       </c>
       <c r="B104" s="1">
-        <v>100228</v>
+        <v>2536669</v>
       </c>
       <c r="C104" s="1">
-        <v>100228</v>
+        <v>2536669</v>
       </c>
       <c r="D104" s="1">
-        <v>100228</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2536669</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2009</v>
       </c>
       <c r="B105" s="1">
-        <v>115157</v>
+        <v>2480756</v>
       </c>
       <c r="C105" s="1">
-        <v>115157</v>
+        <v>2480756</v>
       </c>
       <c r="D105" s="1">
-        <v>115157</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2480756</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2010</v>
       </c>
       <c r="B106" s="1">
-        <v>127334</v>
+        <v>2076297</v>
       </c>
       <c r="C106" s="1">
-        <v>127334</v>
+        <v>2076297</v>
       </c>
       <c r="D106" s="1">
-        <v>127334</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2076297</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2011</v>
       </c>
       <c r="B107" s="1">
-        <v>161968</v>
+        <v>3574922</v>
       </c>
       <c r="C107" s="1">
-        <v>161968</v>
+        <v>3574922</v>
       </c>
       <c r="D107" s="1">
-        <v>161968</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3574922</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>2012</v>
       </c>
       <c r="B108" s="1">
-        <v>66639</v>
+        <v>1158101</v>
       </c>
       <c r="C108" s="1">
-        <v>66639</v>
+        <v>1158101</v>
       </c>
       <c r="D108" s="1">
-        <v>66639</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1158101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>2013</v>
       </c>
       <c r="B109" s="1">
-        <v>112311.0956</v>
+        <v>1738419</v>
       </c>
       <c r="C109" s="1">
-        <v>112311.0956</v>
+        <v>1738419</v>
       </c>
       <c r="D109" s="1">
-        <v>112311.0956</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1738419</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2014</v>
       </c>
       <c r="B110" s="1">
-        <v>161899.80500000002</v>
+        <v>2849181</v>
       </c>
       <c r="C110" s="1">
-        <v>161899.80500000002</v>
+        <v>2849181</v>
       </c>
       <c r="D110" s="1">
-        <v>161899.80500000002</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2849181</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2015</v>
       </c>
       <c r="B111" s="1">
-        <v>172134.41250000001</v>
+        <v>2219415</v>
       </c>
       <c r="C111" s="1">
-        <v>172134.41250000001</v>
+        <v>2219415</v>
       </c>
       <c r="D111" s="1">
-        <v>172134.41250000001</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2219415</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2016</v>
       </c>
       <c r="B112" s="1">
-        <v>109972.06700000001</v>
+        <v>2106977</v>
       </c>
       <c r="C112" s="1">
-        <v>109972.06700000001</v>
+        <v>2106977</v>
       </c>
       <c r="D112" s="1">
-        <v>109972.06700000001</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2106977</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2017</v>
       </c>
       <c r="B113" s="1">
-        <v>139323.94400000002</v>
+        <v>2181450</v>
       </c>
       <c r="C113" s="1">
-        <v>139323.94400000002</v>
+        <v>2181450</v>
       </c>
       <c r="D113" s="1">
-        <v>139323.94400000002</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2181450</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2018</v>
       </c>
       <c r="B114" s="1">
-        <v>83574.923899999994</v>
+        <v>1474316</v>
       </c>
       <c r="C114" s="1">
-        <v>83574.923899999994</v>
+        <v>1474316</v>
       </c>
       <c r="D114" s="1">
-        <v>83574.923899999994</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1474316</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2019</v>
       </c>
       <c r="B115" s="1">
-        <v>121156.83700000001</v>
+        <v>2550862</v>
       </c>
       <c r="C115" s="1">
-        <v>121156.83700000001</v>
+        <v>2550862</v>
       </c>
       <c r="D115" s="1">
-        <v>121156.83700000001</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2550862</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2020</v>
       </c>
       <c r="B116" s="1">
-        <v>90568.119900000005</v>
+        <v>1714823</v>
       </c>
       <c r="C116" s="1">
-        <v>90568.119900000005</v>
+        <v>1714823</v>
       </c>
       <c r="D116" s="1">
-        <v>90568.119900000005</v>
+        <v>1714823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>